<commit_message>
changed trim type for output files
</commit_message>
<xml_diff>
--- a/metadatainjection/metadata/airports_metadata.xlsx
+++ b/metadatainjection/metadata/airports_metadata.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">none</t>
+    <t xml:space="preserve">both</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -207,19 +207,19 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>